<commit_message>
Extracted repeated code into DepthMapUtils.
</commit_message>
<xml_diff>
--- a/paper/timings.xlsx
+++ b/paper/timings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="11112"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="11115"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -315,7 +315,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -462,7 +462,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -558,13 +558,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -581,8 +581,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="217109744"/>
-        <c:axId val="217111984"/>
+        <c:axId val="-1003760496"/>
+        <c:axId val="-1003759952"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -758,7 +758,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="217109744"/>
+        <c:axId val="-1003760496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,7 +786,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -801,7 +801,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217111984"/>
+        <c:crossAx val="-1003759952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -809,7 +809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217111984"/>
+        <c:axId val="-1003759952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -846,7 +846,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -861,7 +861,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217109744"/>
+        <c:crossAx val="-1003760496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -889,7 +889,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1492,15 +1492,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>325755</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>150494</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1788,19 +1788,19 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1865,10 +1865,10 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>3.9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1882,10 +1882,10 @@
         <v>7.9</v>
       </c>
       <c r="E5">
-        <v>32</v>
+        <v>3.9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>27.7</v>
       </c>
       <c r="E6">
-        <v>120</v>
+        <v>3.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>